<commit_message>
Final equity report to be submitted
</commit_message>
<xml_diff>
--- a/vcx_dcf.xlsx
+++ b/vcx_dcf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Documents/FINM3422/Coding Equity Research Report/FM_Equity_Research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Documents/FINM3422/Coding Equity Research Report/Coding Project 1 Repos in Order/FM_Equity_Research-5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A404AD42-26F6-5242-B59C-3A9373561F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE880F28-9312-634E-92DE-347C8FAD173A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{4117CD92-D245-944F-AEE6-67CD9652FC62}"/>
+    <workbookView xWindow="-2360" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{4117CD92-D245-944F-AEE6-67CD9652FC62}"/>
   </bookViews>
   <sheets>
     <sheet name="DCF" sheetId="1" r:id="rId1"/>
@@ -362,7 +362,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="108">
   <si>
     <t xml:space="preserve">Vicinity Centres (ASX: VCX) </t>
   </si>
@@ -673,22 +673,19 @@
     <t xml:space="preserve">EBITDA exit multiple </t>
   </si>
   <si>
-    <t>Weighted Average Cost of Capital (WACC)</t>
-  </si>
-  <si>
-    <t>Terminal Value</t>
-  </si>
-  <si>
-    <t>Enterprise Value</t>
-  </si>
-  <si>
     <t>Equity Value</t>
   </si>
   <si>
-    <t>Shares Outstanding</t>
-  </si>
-  <si>
-    <t>Implied Price</t>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>EV</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Shares Out.</t>
   </si>
 </sst>
 </file>
@@ -1380,8 +1377,8 @@
   <dimension ref="A1:P158"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H155" sqref="H155"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H133" sqref="H133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3102,7 +3099,7 @@
         <v>8.0000000000000016E-2</v>
       </c>
       <c r="H112" s="65">
-        <f t="dataTable" ref="H112:L116" dt2D="1" dtr="1" r1="E18" r2="I11" ca="1"/>
+        <f t="dataTable" ref="H112:L116" dt2D="1" dtr="1" r1="E18" r2="I11"/>
         <v>1.5072312293995938</v>
       </c>
       <c r="I112" s="66">
@@ -3245,7 +3242,7 @@
         <v>0.09</v>
       </c>
       <c r="H121" s="65">
-        <f t="dataTable" ref="H121:L125" dt2D="1" dtr="1" r1="I79" r2="I11"/>
+        <f t="dataTable" ref="H121:L125" dt2D="1" dtr="1" r1="I79" r2="I11" ca="1"/>
         <v>2.0423944487932739</v>
       </c>
       <c r="I121" s="66">
@@ -3680,7 +3677,7 @@
     </row>
     <row r="152" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D152" s="82" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="E152" s="14">
         <v>7.2999999999999995E-2</v>
@@ -3724,7 +3721,7 @@
     </row>
     <row r="156" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D156" s="82" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E156" s="28">
         <v>11100.915456973584</v>
@@ -3746,7 +3743,7 @@
     </row>
     <row r="158" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D158" s="86" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E158" s="87">
         <v>2.4325100697608888</v>

</xml_diff>